<commit_message>
Updates measure to use new logging and new copy model methods
</commit_message>
<xml_diff>
--- a/create_DOE_prototype_building/resources/standards data/HVAC Standards/OpenStudio_HVAC_Standards.xlsx
+++ b/create_DOE_prototype_building/resources/standards data/HVAC Standards/OpenStudio_HVAC_Standards.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="23955" windowHeight="11820" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="30" windowWidth="23955" windowHeight="11820" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="PrototypeInputs" sheetId="1" r:id="rId1"/>
@@ -13,14 +13,16 @@
     <sheet name="CurveBiquadratic" sheetId="3" r:id="rId4"/>
     <sheet name="CurveBicubic" sheetId="4" r:id="rId5"/>
     <sheet name="CurveQuadratic" sheetId="5" r:id="rId6"/>
-    <sheet name="Motors" sheetId="7" r:id="rId7"/>
+    <sheet name="CurveCubic" sheetId="12" r:id="rId7"/>
+    <sheet name="Motors" sheetId="7" r:id="rId8"/>
+    <sheet name="Schedules" sheetId="10" r:id="rId9"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="747" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="926" uniqueCount="195">
   <si>
     <t>Template</t>
   </si>
@@ -428,6 +430,183 @@
   </si>
   <si>
     <t>From 90.1-2004 Table 10.8B</t>
+  </si>
+  <si>
+    <t>Occ Sensing Exterior Lighting Power</t>
+  </si>
+  <si>
+    <t>NonDimming Exterior Lighting Power</t>
+  </si>
+  <si>
+    <t>Water Heater Fuel</t>
+  </si>
+  <si>
+    <t>Electricity</t>
+  </si>
+  <si>
+    <t>Water Heater Volume (gal)</t>
+  </si>
+  <si>
+    <t>Water Heater Capacity (Btu/hr)</t>
+  </si>
+  <si>
+    <t>Service Water Temperature (F)</t>
+  </si>
+  <si>
+    <t>Natural Gas</t>
+  </si>
+  <si>
+    <t>Day Types</t>
+  </si>
+  <si>
+    <t>Start Date</t>
+  </si>
+  <si>
+    <t>End Date</t>
+  </si>
+  <si>
+    <t>From DOE Small Office Prototype Building 90.1-2010</t>
+  </si>
+  <si>
+    <t>Service Water Heating</t>
+  </si>
+  <si>
+    <t>Units</t>
+  </si>
+  <si>
+    <t>Fraction</t>
+  </si>
+  <si>
+    <t>SmallOffice BLDG_SWH_SCH</t>
+  </si>
+  <si>
+    <t>Default, SmrDsn, WntrDsn</t>
+  </si>
+  <si>
+    <t>Wknd, Hol</t>
+  </si>
+  <si>
+    <t>Service Water FlowRate Schedule</t>
+  </si>
+  <si>
+    <t>Hr 1</t>
+  </si>
+  <si>
+    <t>Hr 2</t>
+  </si>
+  <si>
+    <t>Hr 3</t>
+  </si>
+  <si>
+    <t>Hr 4</t>
+  </si>
+  <si>
+    <t>Hr 5</t>
+  </si>
+  <si>
+    <t>Hr 6</t>
+  </si>
+  <si>
+    <t>Hr 7</t>
+  </si>
+  <si>
+    <t>Hr 8</t>
+  </si>
+  <si>
+    <t>Hr 9</t>
+  </si>
+  <si>
+    <t>Hr 10</t>
+  </si>
+  <si>
+    <t>Hr 11</t>
+  </si>
+  <si>
+    <t>Hr 12</t>
+  </si>
+  <si>
+    <t>Hr 13</t>
+  </si>
+  <si>
+    <t>Hr 14</t>
+  </si>
+  <si>
+    <t>Hr 15</t>
+  </si>
+  <si>
+    <t>Hr 16</t>
+  </si>
+  <si>
+    <t>Hr 17</t>
+  </si>
+  <si>
+    <t>Hr 18</t>
+  </si>
+  <si>
+    <t>Hr 19</t>
+  </si>
+  <si>
+    <t>Hr 20</t>
+  </si>
+  <si>
+    <t>Hr 21</t>
+  </si>
+  <si>
+    <t>Hr 22</t>
+  </si>
+  <si>
+    <t>Hr 23</t>
+  </si>
+  <si>
+    <t>Hr 24</t>
+  </si>
+  <si>
+    <t>Day Type choices: Default, Wkdy, Wknd, Mon, Tue, Wed, Thu, Fri, Sat, Sun, WntrDsn, SmrDsn, Hol</t>
+  </si>
+  <si>
+    <t>Service Water Peak FlowRate (gal/min)</t>
+  </si>
+  <si>
+    <t>Water Use Temperature (F)</t>
+  </si>
+  <si>
+    <t>Service Water Temperature at Fixture (F)</t>
+  </si>
+  <si>
+    <t>DOE Ref DX Clg Coil Cool-Cap-fT</t>
+  </si>
+  <si>
+    <t>From DOE Pre-1980 Reference Building</t>
+  </si>
+  <si>
+    <t>DOE Ref DX Clg Coil Cool-EIR-fT</t>
+  </si>
+  <si>
+    <t>DOE Ref DX Clg Coil Cool-PLF-fPLR</t>
+  </si>
+  <si>
+    <t>DOE Ref DX Clg Coil Cool-CAP-fFlow</t>
+  </si>
+  <si>
+    <t>DOE Ref DX Clg Coil Cool-EIR-fFlow</t>
+  </si>
+  <si>
+    <t>COOL-CAP-FT</t>
+  </si>
+  <si>
+    <t>COOL-CAP-FFLOW</t>
+  </si>
+  <si>
+    <t>COOL-EIR-FT</t>
+  </si>
+  <si>
+    <t>COOL-EIR-FFLOW</t>
+  </si>
+  <si>
+    <t>COOL-PLF-FPLR</t>
+  </si>
+  <si>
+    <t>Each row represents a cubic curve used to describe HVAC component performance</t>
   </si>
 </sst>
 </file>
@@ -471,7 +650,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -490,13 +669,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -509,24 +699,165 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="46">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="171" formatCode="m/d"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.0%"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -539,9 +870,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A3:K13" totalsRowShown="0">
-  <autoFilter ref="A3:K13"/>
-  <tableColumns count="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A3:U9" totalsRowShown="0" headerRowDxfId="17">
+  <autoFilter ref="A3:U9"/>
+  <tableColumns count="21">
     <tableColumn id="1" name="Template"/>
     <tableColumn id="2" name="Climate Zone"/>
     <tableColumn id="3" name="BuildingType"/>
@@ -553,6 +884,16 @@
     <tableColumn id="10" name="Unitary AC Cooling Type"/>
     <tableColumn id="11" name="Unitary AC Heating Type"/>
     <tableColumn id="9" name="HX"/>
+    <tableColumn id="12" name="Occ Sensing Exterior Lighting Power"/>
+    <tableColumn id="13" name="NonDimming Exterior Lighting Power"/>
+    <tableColumn id="14" name="Water Heater Volume (gal)"/>
+    <tableColumn id="15" name="Water Heater Fuel"/>
+    <tableColumn id="16" name="Water Heater Capacity (Btu/hr)"/>
+    <tableColumn id="17" name="Service Water Temperature (F)"/>
+    <tableColumn id="18" name="Service Water FlowRate Schedule"/>
+    <tableColumn id="19" name="Service Water Peak FlowRate (gal/min)"/>
+    <tableColumn id="20" name="Water Use Temperature (F)"/>
+    <tableColumn id="21" name="Service Water Temperature at Fixture (F)"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -579,30 +920,32 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table58" displayName="Table58" ref="A3:M63" totalsRowShown="0">
-  <autoFilter ref="A3:M63"/>
-  <tableColumns count="13">
-    <tableColumn id="1" name="Template"/>
-    <tableColumn id="2" name="Cooling Type"/>
-    <tableColumn id="6" name="Heating Type"/>
-    <tableColumn id="8" name="Subcategory"/>
-    <tableColumn id="9" name="Minimum Capacity (Btu/hr)" dataDxfId="3" dataCellStyle="Comma"/>
-    <tableColumn id="7" name="Maximum Capacity (Btu/hr)" dataDxfId="2" dataCellStyle="Comma"/>
-    <tableColumn id="10" name="Minimum SEER"/>
-    <tableColumn id="12" name="Minimum EER"/>
-    <tableColumn id="11" name="Minimum IPLV"/>
-    <tableColumn id="3" name="CAPFT"/>
-    <tableColumn id="4" name="EIRFT"/>
-    <tableColumn id="5" name="EIRFPLR"/>
-    <tableColumn id="13" name="Notes"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table58" displayName="Table58" ref="A3:O63" totalsRowShown="0" headerRowDxfId="2" dataDxfId="16">
+  <autoFilter ref="A3:O63"/>
+  <tableColumns count="15">
+    <tableColumn id="1" name="Template" dataDxfId="15"/>
+    <tableColumn id="2" name="Cooling Type" dataDxfId="14"/>
+    <tableColumn id="6" name="Heating Type" dataDxfId="13"/>
+    <tableColumn id="8" name="Subcategory" dataDxfId="12"/>
+    <tableColumn id="9" name="Minimum Capacity (Btu/hr)" dataDxfId="11" dataCellStyle="Comma"/>
+    <tableColumn id="7" name="Maximum Capacity (Btu/hr)" dataDxfId="10" dataCellStyle="Comma"/>
+    <tableColumn id="10" name="Minimum SEER" dataDxfId="9"/>
+    <tableColumn id="12" name="Minimum EER" dataDxfId="8"/>
+    <tableColumn id="11" name="Minimum IPLV" dataDxfId="7"/>
+    <tableColumn id="3" name="COOL-CAP-FT" dataDxfId="6"/>
+    <tableColumn id="4" name="COOL-CAP-FFLOW" dataDxfId="5"/>
+    <tableColumn id="15" name="COOL-EIR-FT" dataDxfId="0"/>
+    <tableColumn id="14" name="COOL-EIR-FFLOW" dataDxfId="1"/>
+    <tableColumn id="5" name="COOL-PLF-FPLR" dataDxfId="4"/>
+    <tableColumn id="13" name="Notes" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="CurveBiquadraticTable" displayName="CurveBiquadraticTable" ref="A3:L25" totalsRowShown="0">
-  <autoFilter ref="A3:L25"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="CurveBiquadraticTable" displayName="CurveBiquadraticTable" ref="A3:L27" totalsRowShown="0">
+  <autoFilter ref="A3:L27"/>
   <tableColumns count="12">
     <tableColumn id="1" name="Name"/>
     <tableColumn id="2" name="coeff_1"/>
@@ -647,8 +990,8 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="CurveQuadraticTable" displayName="CurveQuadraticTable" ref="A3:G8" totalsRowShown="0">
-  <autoFilter ref="A3:G8"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="CurveQuadraticTable" displayName="CurveQuadraticTable" ref="A3:G9" totalsRowShown="0">
+  <autoFilter ref="A3:G9"/>
   <tableColumns count="7">
     <tableColumn id="1" name="Name"/>
     <tableColumn id="2" name="coeff_1"/>
@@ -663,6 +1006,23 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="CurveCubicTable" displayName="CurveCubicTable" ref="A3:H5" totalsRowShown="0">
+  <autoFilter ref="A3:H5"/>
+  <tableColumns count="8">
+    <tableColumn id="1" name="Name"/>
+    <tableColumn id="2" name="coeff_1"/>
+    <tableColumn id="3" name="coeff_2"/>
+    <tableColumn id="4" name="coeff_3"/>
+    <tableColumn id="5" name="coeff_4"/>
+    <tableColumn id="8" name="min_x"/>
+    <tableColumn id="9" name="max_x"/>
+    <tableColumn id="12" name="notes"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table57" displayName="Table57" ref="A3:G69" totalsRowShown="0">
   <autoFilter ref="A3:G69"/>
   <tableColumns count="7">
@@ -670,9 +1030,49 @@
     <tableColumn id="2" name="Number of Poles"/>
     <tableColumn id="6" name="Type"/>
     <tableColumn id="9" name="Minimum Capacity (HP)"/>
-    <tableColumn id="7" name="Maximum Capacity (HP)" dataDxfId="1"/>
-    <tableColumn id="10" name="Nominal Full Load Efficiency" dataDxfId="0" dataCellStyle="Percent"/>
+    <tableColumn id="7" name="Maximum Capacity (HP)" dataDxfId="45"/>
+    <tableColumn id="10" name="Nominal Full Load Efficiency" dataDxfId="44" dataCellStyle="Percent"/>
     <tableColumn id="5" name="Notes"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table579" displayName="Table579" ref="A3:AE5" totalsRowShown="0">
+  <autoFilter ref="A3:AE5"/>
+  <tableColumns count="31">
+    <tableColumn id="1" name="Name"/>
+    <tableColumn id="2" name="Type"/>
+    <tableColumn id="31" name="Units"/>
+    <tableColumn id="6" name="Day Types"/>
+    <tableColumn id="9" name="Start Date" dataDxfId="43"/>
+    <tableColumn id="7" name="End Date" dataDxfId="42"/>
+    <tableColumn id="10" name="Hr 1" dataDxfId="41" dataCellStyle="Percent"/>
+    <tableColumn id="5" name="Hr 2" dataDxfId="40" dataCellStyle="Percent"/>
+    <tableColumn id="3" name="Hr 3" dataDxfId="39" dataCellStyle="Percent"/>
+    <tableColumn id="4" name="Hr 4" dataDxfId="38" dataCellStyle="Percent"/>
+    <tableColumn id="8" name="Hr 5" dataDxfId="37" dataCellStyle="Percent"/>
+    <tableColumn id="11" name="Hr 6" dataDxfId="36" dataCellStyle="Percent"/>
+    <tableColumn id="12" name="Hr 7" dataDxfId="35" dataCellStyle="Percent"/>
+    <tableColumn id="13" name="Hr 8" dataDxfId="34" dataCellStyle="Percent"/>
+    <tableColumn id="14" name="Hr 9" dataDxfId="33" dataCellStyle="Percent"/>
+    <tableColumn id="15" name="Hr 10" dataDxfId="32" dataCellStyle="Percent"/>
+    <tableColumn id="16" name="Hr 11" dataDxfId="31" dataCellStyle="Percent"/>
+    <tableColumn id="17" name="Hr 12" dataDxfId="30" dataCellStyle="Percent"/>
+    <tableColumn id="18" name="Hr 13" dataDxfId="29" dataCellStyle="Percent"/>
+    <tableColumn id="19" name="Hr 14" dataDxfId="28" dataCellStyle="Percent"/>
+    <tableColumn id="20" name="Hr 15" dataDxfId="27" dataCellStyle="Percent"/>
+    <tableColumn id="21" name="Hr 16" dataDxfId="26" dataCellStyle="Percent"/>
+    <tableColumn id="22" name="Hr 17" dataDxfId="25" dataCellStyle="Percent"/>
+    <tableColumn id="23" name="Hr 18" dataDxfId="24" dataCellStyle="Percent"/>
+    <tableColumn id="24" name="Hr 19" dataDxfId="23" dataCellStyle="Percent"/>
+    <tableColumn id="25" name="Hr 20" dataDxfId="22" dataCellStyle="Percent"/>
+    <tableColumn id="26" name="Hr 21" dataDxfId="21" dataCellStyle="Percent"/>
+    <tableColumn id="27" name="Hr 22" dataDxfId="20" dataCellStyle="Percent"/>
+    <tableColumn id="28" name="Hr 23" dataDxfId="19" dataCellStyle="Percent"/>
+    <tableColumn id="29" name="Hr 24" dataDxfId="18" dataCellStyle="Percent"/>
+    <tableColumn id="30" name="Notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -965,13 +1365,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:U9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A8" sqref="A8"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="N4" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight" activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -987,14 +1387,23 @@
     <col min="9" max="9" width="27.5703125" customWidth="1"/>
     <col min="10" max="10" width="25.42578125" customWidth="1"/>
     <col min="11" max="11" width="11.5703125" customWidth="1"/>
+    <col min="12" max="12" width="37.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="38.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.140625" customWidth="1"/>
+    <col min="17" max="17" width="13" customWidth="1"/>
+    <col min="18" max="18" width="26.140625" customWidth="1"/>
+    <col min="19" max="19" width="14.7109375" customWidth="1"/>
+    <col min="20" max="20" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" s="4" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -1004,32 +1413,62 @@
       <c r="C3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" s="4" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L3" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="P3" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="Q3" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="R3" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="S3" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="T3" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="U3" s="4" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1058,7 +1497,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1087,7 +1526,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
@@ -1119,7 +1558,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -1138,8 +1577,35 @@
       <c r="K7" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M7">
+        <v>2766</v>
+      </c>
+      <c r="N7">
+        <v>40</v>
+      </c>
+      <c r="O7" t="s">
+        <v>143</v>
+      </c>
+      <c r="P7" s="6">
+        <v>2883000</v>
+      </c>
+      <c r="Q7">
+        <v>140</v>
+      </c>
+      <c r="R7" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="S7">
+        <v>0.05</v>
+      </c>
+      <c r="T7">
+        <v>110</v>
+      </c>
+      <c r="U7">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1158,8 +1624,35 @@
       <c r="K8" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M8">
+        <v>2766</v>
+      </c>
+      <c r="N8">
+        <v>40</v>
+      </c>
+      <c r="O8" t="s">
+        <v>143</v>
+      </c>
+      <c r="P8" s="6">
+        <v>2883000</v>
+      </c>
+      <c r="Q8">
+        <v>140</v>
+      </c>
+      <c r="R8" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="S8" s="8">
+        <v>0.05</v>
+      </c>
+      <c r="T8" s="8">
+        <v>110</v>
+      </c>
+      <c r="U8" s="8">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>2</v>
       </c>
@@ -1177,6 +1670,36 @@
       </c>
       <c r="K9" t="b">
         <v>0</v>
+      </c>
+      <c r="L9">
+        <v>896.07</v>
+      </c>
+      <c r="M9">
+        <v>40.54</v>
+      </c>
+      <c r="N9">
+        <v>40</v>
+      </c>
+      <c r="O9" t="s">
+        <v>139</v>
+      </c>
+      <c r="P9" s="6">
+        <v>40000</v>
+      </c>
+      <c r="Q9" s="8">
+        <v>140</v>
+      </c>
+      <c r="R9" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="S9">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="T9">
+        <v>120</v>
+      </c>
+      <c r="U9">
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -1192,10 +1715,10 @@
   <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="6" ySplit="3" topLeftCell="I4" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G1" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="F37" sqref="F37"/>
+      <pane xSplit="6" ySplit="3" topLeftCell="G4" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight" activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1598,13 +2121,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M63"/>
+  <dimension ref="A1:O73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="6" ySplit="3" topLeftCell="G4" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G1" sqref="G1"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="5" ySplit="3" topLeftCell="F4" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A22" sqref="A22"/>
+      <selection pane="bottomRight" activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1615,20 +2138,21 @@
     <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="21.7109375" customWidth="1"/>
-    <col min="9" max="9" width="24" customWidth="1"/>
-    <col min="10" max="10" width="66" customWidth="1"/>
-    <col min="11" max="11" width="65" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="70.7109375" customWidth="1"/>
-    <col min="13" max="13" width="36.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="28.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="32.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="36.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" s="4" customFormat="1" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
@@ -1647,1520 +2171,1842 @@
       <c r="F3" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="J3" t="s">
-        <v>79</v>
-      </c>
-      <c r="K3" t="s">
-        <v>80</v>
-      </c>
-      <c r="L3" t="s">
-        <v>81</v>
-      </c>
-      <c r="M3" t="s">
+      <c r="J3" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="O3" s="4" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:15" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="E4" s="6">
-        <v>0</v>
-      </c>
-      <c r="F4" s="6">
+      <c r="E4" s="14">
+        <v>0</v>
+      </c>
+      <c r="F4" s="14">
         <v>64999</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="13">
         <v>11.09</v>
       </c>
-      <c r="M4" t="s">
+      <c r="J4" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="K4" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="L4" s="13" t="s">
+        <v>185</v>
+      </c>
+      <c r="M4" s="13" t="s">
+        <v>188</v>
+      </c>
+      <c r="N4" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="O4" s="13" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:15" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="E5" s="6">
-        <v>0</v>
-      </c>
-      <c r="F5" s="6">
+      <c r="E5" s="14">
+        <v>0</v>
+      </c>
+      <c r="F5" s="14">
         <v>64999</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="13">
         <v>11.09</v>
       </c>
-      <c r="M5" t="s">
+      <c r="J5" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="K5" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="L5" s="13" t="s">
+        <v>185</v>
+      </c>
+      <c r="M5" s="13" t="s">
+        <v>188</v>
+      </c>
+      <c r="N5" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="O5" s="13" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:15" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="E6" s="6">
-        <v>0</v>
-      </c>
-      <c r="F6" s="6">
+      <c r="E6" s="14">
+        <v>0</v>
+      </c>
+      <c r="F6" s="14">
         <v>64999</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="13">
         <v>11.06</v>
       </c>
-      <c r="M6" t="s">
+      <c r="J6" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="K6" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="L6" s="13" t="s">
+        <v>185</v>
+      </c>
+      <c r="M6" s="13" t="s">
+        <v>188</v>
+      </c>
+      <c r="N6" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="O6" s="13" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="1:15" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="E7" s="6">
-        <v>0</v>
-      </c>
-      <c r="F7" s="6">
+      <c r="E7" s="14">
+        <v>0</v>
+      </c>
+      <c r="F7" s="14">
         <v>64999</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="13">
         <v>11.06</v>
       </c>
-      <c r="M7" t="s">
+      <c r="J7" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="K7" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="L7" s="13" t="s">
+        <v>185</v>
+      </c>
+      <c r="M7" s="13" t="s">
+        <v>188</v>
+      </c>
+      <c r="N7" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="O7" s="13" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="8" spans="1:15" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="14">
         <v>65000</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="14">
         <v>134999</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="13">
         <v>9.6300000000000008</v>
       </c>
-      <c r="M8" t="s">
+      <c r="J8" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="K8" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="L8" s="13" t="s">
+        <v>185</v>
+      </c>
+      <c r="M8" s="13" t="s">
+        <v>188</v>
+      </c>
+      <c r="N8" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="O8" s="13" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="9" spans="1:15" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="14">
         <v>65000</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F9" s="14">
         <v>134999</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="13">
         <v>9.6300000000000008</v>
       </c>
-      <c r="M9" t="s">
+      <c r="J9" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="K9" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="L9" s="13" t="s">
+        <v>185</v>
+      </c>
+      <c r="M9" s="13" t="s">
+        <v>188</v>
+      </c>
+      <c r="N9" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="O9" s="13" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="10" spans="1:15" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="14">
         <v>65000</v>
       </c>
-      <c r="F10" s="6">
+      <c r="F10" s="14">
         <v>134999</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="13">
         <v>9.6300000000000008</v>
       </c>
-      <c r="M10" t="s">
+      <c r="J10" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="K10" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="L10" s="13" t="s">
+        <v>185</v>
+      </c>
+      <c r="M10" s="13" t="s">
+        <v>188</v>
+      </c>
+      <c r="N10" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="O10" s="13" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="11" spans="1:15" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="14">
         <v>65000</v>
       </c>
-      <c r="F11" s="6">
+      <c r="F11" s="14">
         <v>134999</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="13">
         <v>9.6300000000000008</v>
       </c>
-      <c r="M11" t="s">
+      <c r="J11" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="K11" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="L11" s="13" t="s">
+        <v>185</v>
+      </c>
+      <c r="M11" s="13" t="s">
+        <v>188</v>
+      </c>
+      <c r="N11" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="O11" s="13" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="12" spans="1:15" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="14">
         <v>135000</v>
       </c>
-      <c r="F12" s="6">
+      <c r="F12" s="14">
         <v>239999</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="13">
         <v>9.2799999999999994</v>
       </c>
-      <c r="M12" t="s">
+      <c r="J12" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="K12" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="L12" s="13" t="s">
+        <v>185</v>
+      </c>
+      <c r="M12" s="13" t="s">
+        <v>188</v>
+      </c>
+      <c r="N12" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="O12" s="13" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="13" spans="1:15" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="E13" s="6">
+      <c r="E13" s="14">
         <v>135000</v>
       </c>
-      <c r="F13" s="6">
+      <c r="F13" s="14">
         <v>239999</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="13">
         <v>9.2799999999999994</v>
       </c>
-      <c r="M13" t="s">
+      <c r="J13" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="K13" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="L13" s="13" t="s">
+        <v>185</v>
+      </c>
+      <c r="M13" s="13" t="s">
+        <v>188</v>
+      </c>
+      <c r="N13" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="O13" s="13" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="14" spans="1:15" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="E14" s="6">
+      <c r="E14" s="14">
         <v>135000</v>
       </c>
-      <c r="F14" s="6">
+      <c r="F14" s="14">
         <v>239999</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="13">
         <v>9.2799999999999994</v>
       </c>
-      <c r="M14" t="s">
+      <c r="J14" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="K14" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="L14" s="13" t="s">
+        <v>185</v>
+      </c>
+      <c r="M14" s="13" t="s">
+        <v>188</v>
+      </c>
+      <c r="N14" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="O14" s="13" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="15" spans="1:15" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="E15" s="6">
+      <c r="E15" s="14">
         <v>135000</v>
       </c>
-      <c r="F15" s="6">
+      <c r="F15" s="14">
         <v>239999</v>
       </c>
-      <c r="H15">
+      <c r="H15" s="13">
         <v>9.2799999999999994</v>
       </c>
-      <c r="M15" t="s">
+      <c r="J15" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="K15" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="L15" s="13" t="s">
+        <v>185</v>
+      </c>
+      <c r="M15" s="13" t="s">
+        <v>188</v>
+      </c>
+      <c r="N15" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="O15" s="13" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="16" spans="1:15" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="E16" s="6">
+      <c r="E16" s="14">
         <v>240000</v>
       </c>
-      <c r="F16" s="6">
+      <c r="F16" s="14">
         <v>759999</v>
       </c>
-      <c r="H16">
+      <c r="H16" s="13">
         <v>8.92</v>
       </c>
-      <c r="M16" t="s">
+      <c r="J16" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="K16" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="L16" s="13" t="s">
+        <v>185</v>
+      </c>
+      <c r="M16" s="13" t="s">
+        <v>188</v>
+      </c>
+      <c r="N16" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="O16" s="13" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="17" spans="1:15" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="E17" s="6">
+      <c r="E17" s="14">
         <v>240000</v>
       </c>
-      <c r="F17" s="6">
+      <c r="F17" s="14">
         <v>759999</v>
       </c>
-      <c r="H17">
+      <c r="H17" s="13">
         <v>8.92</v>
       </c>
-      <c r="M17" t="s">
+      <c r="J17" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="K17" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="L17" s="13" t="s">
+        <v>185</v>
+      </c>
+      <c r="M17" s="13" t="s">
+        <v>188</v>
+      </c>
+      <c r="N17" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="O17" s="13" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="18" spans="1:15" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="E18" s="6">
+      <c r="E18" s="14">
         <v>240000</v>
       </c>
-      <c r="F18" s="6">
+      <c r="F18" s="14">
         <v>759999</v>
       </c>
-      <c r="H18">
+      <c r="H18" s="13">
         <v>8.92</v>
       </c>
-      <c r="M18" t="s">
+      <c r="J18" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="K18" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="L18" s="13" t="s">
+        <v>185</v>
+      </c>
+      <c r="M18" s="13" t="s">
+        <v>188</v>
+      </c>
+      <c r="N18" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="O18" s="13" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="19" spans="1:15" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="E19" s="6">
+      <c r="E19" s="14">
         <v>240000</v>
       </c>
-      <c r="F19" s="6">
+      <c r="F19" s="14">
         <v>759999</v>
       </c>
-      <c r="H19">
+      <c r="H19" s="13">
         <v>8.92</v>
       </c>
-      <c r="M19" t="s">
+      <c r="J19" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="K19" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="L19" s="13" t="s">
+        <v>185</v>
+      </c>
+      <c r="M19" s="13" t="s">
+        <v>188</v>
+      </c>
+      <c r="N19" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="O19" s="13" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="20" spans="1:15" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="E20" s="6">
+      <c r="E20" s="14">
         <v>760000</v>
       </c>
-      <c r="F20" s="6">
+      <c r="F20" s="14">
         <v>9999999</v>
       </c>
-      <c r="H20">
+      <c r="H20" s="13">
         <v>8.6300000000000008</v>
       </c>
-      <c r="M20" t="s">
+      <c r="J20" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="K20" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="L20" s="13" t="s">
+        <v>185</v>
+      </c>
+      <c r="M20" s="13" t="s">
+        <v>188</v>
+      </c>
+      <c r="N20" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="O20" s="13" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="21" spans="1:15" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="E21" s="6">
+      <c r="E21" s="14">
         <v>760000</v>
       </c>
-      <c r="F21" s="6">
+      <c r="F21" s="14">
         <v>9999999</v>
       </c>
-      <c r="H21">
+      <c r="H21" s="13">
         <v>8.6300000000000008</v>
       </c>
-      <c r="M21" t="s">
+      <c r="J21" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="K21" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="L21" s="13" t="s">
+        <v>185</v>
+      </c>
+      <c r="M21" s="13" t="s">
+        <v>188</v>
+      </c>
+      <c r="N21" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="O21" s="13" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="22" spans="1:15" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="E22" s="6">
+      <c r="E22" s="14">
         <v>760000</v>
       </c>
-      <c r="F22" s="6">
+      <c r="F22" s="14">
         <v>9999999</v>
       </c>
-      <c r="H22">
+      <c r="H22" s="13">
         <v>8.6300000000000008</v>
       </c>
-      <c r="M22" t="s">
+      <c r="J22" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="K22" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="L22" s="13" t="s">
+        <v>185</v>
+      </c>
+      <c r="M22" s="13" t="s">
+        <v>188</v>
+      </c>
+      <c r="N22" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="O22" s="13" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="23" spans="1:15" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="E23" s="6">
+      <c r="E23" s="14">
         <v>760000</v>
       </c>
-      <c r="F23" s="6">
+      <c r="F23" s="14">
         <v>9999999</v>
       </c>
-      <c r="H23">
+      <c r="H23" s="13">
         <v>8.6300000000000008</v>
       </c>
-      <c r="M23" t="s">
+      <c r="J23" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="K23" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="L23" s="13" t="s">
+        <v>185</v>
+      </c>
+      <c r="M23" s="13" t="s">
+        <v>188</v>
+      </c>
+      <c r="N23" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="O23" s="13" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="24" spans="1:15" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="E24" s="6">
-        <v>0</v>
-      </c>
-      <c r="F24" s="6">
+      <c r="E24" s="14">
+        <v>0</v>
+      </c>
+      <c r="F24" s="14">
         <v>64999</v>
       </c>
-      <c r="G24">
+      <c r="G24" s="13">
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="25" spans="1:15" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="E25" s="6">
-        <v>0</v>
-      </c>
-      <c r="F25" s="6">
+      <c r="E25" s="14">
+        <v>0</v>
+      </c>
+      <c r="F25" s="14">
         <v>64999</v>
       </c>
-      <c r="G25">
+      <c r="G25" s="13">
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="26" spans="1:15" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="E26" s="6">
-        <v>0</v>
-      </c>
-      <c r="F26" s="6">
+      <c r="E26" s="14">
+        <v>0</v>
+      </c>
+      <c r="F26" s="14">
         <v>64999</v>
       </c>
-      <c r="G26">
+      <c r="G26" s="13">
         <v>9.6999999999999993</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="27" spans="1:15" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="E27" s="6">
-        <v>0</v>
-      </c>
-      <c r="F27" s="6">
+      <c r="E27" s="14">
+        <v>0</v>
+      </c>
+      <c r="F27" s="14">
         <v>64999</v>
       </c>
-      <c r="G27">
+      <c r="G27" s="13">
         <v>9.6999999999999993</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="28" spans="1:15" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="E28" s="6">
+      <c r="E28" s="14">
         <v>65000</v>
       </c>
-      <c r="F28" s="6">
+      <c r="F28" s="14">
         <v>134999</v>
       </c>
-      <c r="H28">
+      <c r="H28" s="13">
         <v>10.3</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="29" spans="1:15" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="E29" s="6">
+      <c r="E29" s="14">
         <v>65000</v>
       </c>
-      <c r="F29" s="6">
+      <c r="F29" s="14">
         <v>134999</v>
       </c>
-      <c r="H29">
+      <c r="H29" s="13">
         <v>10.3</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="30" spans="1:15" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="E30" s="6">
+      <c r="E30" s="14">
         <v>65000</v>
       </c>
-      <c r="F30" s="6">
+      <c r="F30" s="14">
         <v>134999</v>
       </c>
-      <c r="H30">
+      <c r="H30" s="13">
         <v>10.1</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+    <row r="31" spans="1:15" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="E31" s="6">
+      <c r="E31" s="14">
         <v>65000</v>
       </c>
-      <c r="F31" s="6">
+      <c r="F31" s="14">
         <v>134999</v>
       </c>
-      <c r="H31">
+      <c r="H31" s="13">
         <v>10.1</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+    <row r="32" spans="1:15" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D32" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="E32" s="6">
+      <c r="E32" s="14">
         <v>135000</v>
       </c>
-      <c r="F32" s="6">
+      <c r="F32" s="14">
         <v>239999</v>
       </c>
-      <c r="H32">
+      <c r="H32" s="13">
         <v>9.6999999999999993</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="33" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D33" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="E33" s="6">
+      <c r="E33" s="14">
         <v>135000</v>
       </c>
-      <c r="F33" s="6">
+      <c r="F33" s="14">
         <v>239999</v>
       </c>
-      <c r="H33">
+      <c r="H33" s="13">
         <v>9.6999999999999993</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="34" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D34" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="E34" s="6">
+      <c r="E34" s="14">
         <v>135000</v>
       </c>
-      <c r="F34" s="6">
+      <c r="F34" s="14">
         <v>239999</v>
       </c>
-      <c r="H34">
+      <c r="H34" s="13">
         <v>9.5</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+    <row r="35" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D35" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="E35" s="6">
+      <c r="E35" s="14">
         <v>135000</v>
       </c>
-      <c r="F35" s="6">
+      <c r="F35" s="14">
         <v>239999</v>
       </c>
-      <c r="H35">
+      <c r="H35" s="13">
         <v>9.5</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+    <row r="36" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D36" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="E36" s="6">
+      <c r="E36" s="14">
         <v>240000</v>
       </c>
-      <c r="F36" s="6">
+      <c r="F36" s="14">
         <v>759999</v>
       </c>
-      <c r="H36">
+      <c r="H36" s="13">
         <v>9.5</v>
       </c>
-      <c r="I36">
+      <c r="I36" s="13">
         <v>9.6999999999999993</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+    <row r="37" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D37" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="E37" s="6">
+      <c r="E37" s="14">
         <v>240000</v>
       </c>
-      <c r="F37" s="6">
+      <c r="F37" s="14">
         <v>759999</v>
       </c>
-      <c r="H37">
+      <c r="H37" s="13">
         <v>9.5</v>
       </c>
-      <c r="I37">
+      <c r="I37" s="13">
         <v>9.6999999999999993</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    <row r="38" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D38" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="E38" s="6">
+      <c r="E38" s="14">
         <v>240000</v>
       </c>
-      <c r="F38" s="6">
+      <c r="F38" s="14">
         <v>759999</v>
       </c>
-      <c r="H38">
+      <c r="H38" s="13">
         <v>9.3000000000000007</v>
       </c>
-      <c r="I38">
+      <c r="I38" s="13">
         <v>9.5</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+    <row r="39" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D39" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="E39" s="6">
+      <c r="E39" s="14">
         <v>240000</v>
       </c>
-      <c r="F39" s="6">
+      <c r="F39" s="14">
         <v>759999</v>
       </c>
-      <c r="H39">
+      <c r="H39" s="13">
         <v>9.3000000000000007</v>
       </c>
-      <c r="I39">
+      <c r="I39" s="13">
         <v>9.5</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+    <row r="40" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C40" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D40" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="E40" s="6">
+      <c r="E40" s="14">
         <v>760000</v>
       </c>
-      <c r="F40" s="6">
+      <c r="F40" s="14">
         <v>9999999</v>
       </c>
-      <c r="H40">
+      <c r="H40" s="13">
         <v>9.1999999999999993</v>
       </c>
-      <c r="I40">
+      <c r="I40" s="13">
         <v>9.4</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+    <row r="41" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C41" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D41" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="E41" s="6">
+      <c r="E41" s="14">
         <v>760000</v>
       </c>
-      <c r="F41" s="6">
+      <c r="F41" s="14">
         <v>9999999</v>
       </c>
-      <c r="H41">
+      <c r="H41" s="13">
         <v>9.1999999999999993</v>
       </c>
-      <c r="I41">
+      <c r="I41" s="13">
         <v>9.4</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+    <row r="42" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C42" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D42" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="E42" s="6">
+      <c r="E42" s="14">
         <v>760000</v>
       </c>
-      <c r="F42" s="6">
+      <c r="F42" s="14">
         <v>9999999</v>
       </c>
-      <c r="H42">
+      <c r="H42" s="13">
         <v>9</v>
       </c>
-      <c r="I42">
+      <c r="I42" s="13">
         <v>9.1999999999999993</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+    <row r="43" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C43" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D43" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="E43" s="6">
+      <c r="E43" s="14">
         <v>760000</v>
       </c>
-      <c r="F43" s="6">
+      <c r="F43" s="14">
         <v>9999999</v>
       </c>
-      <c r="H43">
+      <c r="H43" s="13">
         <v>9</v>
       </c>
-      <c r="I43">
+      <c r="I43" s="13">
         <v>9.1999999999999993</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+    <row r="44" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C44" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D44" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="E44" s="6">
-        <v>0</v>
-      </c>
-      <c r="F44" s="6">
+      <c r="E44" s="14">
+        <v>0</v>
+      </c>
+      <c r="F44" s="14">
         <v>64999</v>
       </c>
-      <c r="G44">
+      <c r="G44" s="13">
         <v>13</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+    <row r="45" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B45" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C45" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D45" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="E45" s="6">
-        <v>0</v>
-      </c>
-      <c r="F45" s="6">
+      <c r="E45" s="14">
+        <v>0</v>
+      </c>
+      <c r="F45" s="14">
         <v>64999</v>
       </c>
-      <c r="G45">
+      <c r="G45" s="13">
         <v>13</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+    <row r="46" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B46" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C46" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D46" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="E46" s="6">
-        <v>0</v>
-      </c>
-      <c r="F46" s="6">
+      <c r="E46" s="14">
+        <v>0</v>
+      </c>
+      <c r="F46" s="14">
         <v>64999</v>
       </c>
-      <c r="G46">
+      <c r="G46" s="13">
         <v>13</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+    <row r="47" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C47" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D47" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="E47" s="6">
-        <v>0</v>
-      </c>
-      <c r="F47" s="6">
+      <c r="E47" s="14">
+        <v>0</v>
+      </c>
+      <c r="F47" s="14">
         <v>64999</v>
       </c>
-      <c r="G47">
+      <c r="G47" s="13">
         <v>13</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+    <row r="48" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C48" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D48" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="E48" s="6">
+      <c r="E48" s="14">
         <v>65000</v>
       </c>
-      <c r="F48" s="6">
+      <c r="F48" s="14">
         <v>134999</v>
       </c>
-      <c r="H48">
+      <c r="H48" s="13">
         <v>11.2</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+    <row r="49" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C49" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D49" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="E49" s="6">
+      <c r="E49" s="14">
         <v>65000</v>
       </c>
-      <c r="F49" s="6">
+      <c r="F49" s="14">
         <v>134999</v>
       </c>
-      <c r="H49">
+      <c r="H49" s="13">
         <v>11.2</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+    <row r="50" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B50" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C50" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D50" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="E50" s="6">
+      <c r="E50" s="14">
         <v>65000</v>
       </c>
-      <c r="F50" s="6">
+      <c r="F50" s="14">
         <v>134999</v>
       </c>
-      <c r="H50">
+      <c r="H50" s="13">
         <v>11</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+    <row r="51" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B51" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C51" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="D51" t="s">
+      <c r="D51" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="E51" s="6">
+      <c r="E51" s="14">
         <v>65000</v>
       </c>
-      <c r="F51" s="6">
+      <c r="F51" s="14">
         <v>134999</v>
       </c>
-      <c r="H51">
+      <c r="H51" s="13">
         <v>11</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+    <row r="52" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B52" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C52" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="D52" t="s">
+      <c r="D52" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="E52" s="6">
+      <c r="E52" s="14">
         <v>135000</v>
       </c>
-      <c r="F52" s="6">
+      <c r="F52" s="14">
         <v>239999</v>
       </c>
-      <c r="H52">
+      <c r="H52" s="13">
         <v>11</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+    <row r="53" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B53" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C53" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="D53" t="s">
+      <c r="D53" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="E53" s="6">
+      <c r="E53" s="14">
         <v>135000</v>
       </c>
-      <c r="F53" s="6">
+      <c r="F53" s="14">
         <v>239999</v>
       </c>
-      <c r="H53">
+      <c r="H53" s="13">
         <v>11</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+    <row r="54" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B54" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C54" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="D54" t="s">
+      <c r="D54" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="E54" s="6">
+      <c r="E54" s="14">
         <v>135000</v>
       </c>
-      <c r="F54" s="6">
+      <c r="F54" s="14">
         <v>239999</v>
       </c>
-      <c r="H54">
+      <c r="H54" s="13">
         <v>10.8</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+    <row r="55" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B55" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C55" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="D55" t="s">
+      <c r="D55" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="E55" s="6">
+      <c r="E55" s="14">
         <v>135000</v>
       </c>
-      <c r="F55" s="6">
+      <c r="F55" s="14">
         <v>239999</v>
       </c>
-      <c r="H55">
+      <c r="H55" s="13">
         <v>10.8</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+    <row r="56" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B56" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C56" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="D56" t="s">
+      <c r="D56" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="E56" s="6">
+      <c r="E56" s="14">
         <v>240000</v>
       </c>
-      <c r="F56" s="6">
+      <c r="F56" s="14">
         <v>759999</v>
       </c>
-      <c r="H56">
+      <c r="H56" s="13">
         <v>10</v>
       </c>
-      <c r="I56">
+      <c r="I56" s="13">
         <v>9.6999999999999993</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+    <row r="57" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B57" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C57" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="D57" t="s">
+      <c r="D57" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="E57" s="6">
+      <c r="E57" s="14">
         <v>240000</v>
       </c>
-      <c r="F57" s="6">
+      <c r="F57" s="14">
         <v>759999</v>
       </c>
-      <c r="H57">
+      <c r="H57" s="13">
         <v>10</v>
       </c>
-      <c r="I57">
+      <c r="I57" s="13">
         <v>9.6999999999999993</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
+    <row r="58" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B58" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C58" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="D58" t="s">
+      <c r="D58" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="E58" s="6">
+      <c r="E58" s="14">
         <v>240000</v>
       </c>
-      <c r="F58" s="6">
+      <c r="F58" s="14">
         <v>759999</v>
       </c>
-      <c r="H58">
+      <c r="H58" s="13">
         <v>9.8000000000000007</v>
       </c>
-      <c r="I58">
+      <c r="I58" s="13">
         <v>9.6999999999999993</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+    <row r="59" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B59" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C59" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="D59" t="s">
+      <c r="D59" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="E59" s="6">
+      <c r="E59" s="14">
         <v>240000</v>
       </c>
-      <c r="F59" s="6">
+      <c r="F59" s="14">
         <v>759999</v>
       </c>
-      <c r="H59">
+      <c r="H59" s="13">
         <v>9.8000000000000007</v>
       </c>
-      <c r="I59">
+      <c r="I59" s="13">
         <v>9.6999999999999993</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
+    <row r="60" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B60" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C60" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="D60" t="s">
+      <c r="D60" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="E60" s="6">
+      <c r="E60" s="14">
         <v>760000</v>
       </c>
-      <c r="F60" s="6">
+      <c r="F60" s="14">
         <v>9999999</v>
       </c>
-      <c r="H60">
+      <c r="H60" s="13">
         <v>9.6999999999999993</v>
       </c>
-      <c r="I60">
+      <c r="I60" s="13">
         <v>9.4</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
+    <row r="61" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B61" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C61" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="D61" t="s">
+      <c r="D61" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="E61" s="6">
+      <c r="E61" s="14">
         <v>760000</v>
       </c>
-      <c r="F61" s="6">
+      <c r="F61" s="14">
         <v>9999999</v>
       </c>
-      <c r="H61">
+      <c r="H61" s="13">
         <v>9.6999999999999993</v>
       </c>
-      <c r="I61">
+      <c r="I61" s="13">
         <v>9.4</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
+    <row r="62" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B62" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C62" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="D62" t="s">
+      <c r="D62" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="E62" s="6">
+      <c r="E62" s="14">
         <v>760000</v>
       </c>
-      <c r="F62" s="6">
+      <c r="F62" s="14">
         <v>9999999</v>
       </c>
-      <c r="H62">
+      <c r="H62" s="13">
         <v>9.5</v>
       </c>
-      <c r="I62">
+      <c r="I62" s="13">
         <v>9.1999999999999993</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
+    <row r="63" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B63" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C63" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="D63" t="s">
+      <c r="D63" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="E63" s="6">
+      <c r="E63" s="14">
         <v>760000</v>
       </c>
-      <c r="F63" s="6">
+      <c r="F63" s="14">
         <v>9999999</v>
       </c>
-      <c r="H63">
+      <c r="H63" s="13">
         <v>9.5</v>
       </c>
-      <c r="I63">
+      <c r="I63" s="13">
         <v>9.1999999999999993</v>
       </c>
     </row>
+    <row r="64" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="65" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="66" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="67" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="68" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="69" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="70" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="71" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="72" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="73" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <dataValidations disablePrompts="1" count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J4:K63">
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J4:J63 L4:L63">
       <formula1>INDIRECT("CurveBiquadraticTable[Name]")</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K4:K63 M4:M63">
+      <formula1>INDIRECT("CurveCubicTable[Name]")</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N4:N63">
+      <formula1>INDIRECT("CurveQuadraticTable[Name]")</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3172,10 +4018,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L25"/>
+  <dimension ref="A1:L27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+      <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4065,6 +4911,82 @@
         <v>47</v>
       </c>
     </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>183</v>
+      </c>
+      <c r="B26">
+        <v>0.97121230000000003</v>
+      </c>
+      <c r="C26">
+        <v>-1.5275502E-2</v>
+      </c>
+      <c r="D26">
+        <v>1.4434523999999999E-3</v>
+      </c>
+      <c r="E26">
+        <v>-3.9321000000000001E-4</v>
+      </c>
+      <c r="F26">
+        <v>-6.8364000000000003E-6</v>
+      </c>
+      <c r="G26">
+        <v>-2.9059559999999998E-4</v>
+      </c>
+      <c r="H26">
+        <v>-100</v>
+      </c>
+      <c r="I26">
+        <v>100</v>
+      </c>
+      <c r="J26">
+        <v>-100</v>
+      </c>
+      <c r="K26">
+        <v>100</v>
+      </c>
+      <c r="L26" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>185</v>
+      </c>
+      <c r="B27">
+        <v>0.28687132999999998</v>
+      </c>
+      <c r="C27">
+        <v>2.3902164E-2</v>
+      </c>
+      <c r="D27">
+        <v>-8.1064799999999997E-4</v>
+      </c>
+      <c r="E27">
+        <v>1.3458546E-2</v>
+      </c>
+      <c r="F27">
+        <v>3.389364E-4</v>
+      </c>
+      <c r="G27">
+        <v>-4.870044E-4</v>
+      </c>
+      <c r="H27" s="8">
+        <v>-100</v>
+      </c>
+      <c r="I27" s="8">
+        <v>100</v>
+      </c>
+      <c r="J27" s="8">
+        <v>-100</v>
+      </c>
+      <c r="K27" s="8">
+        <v>100</v>
+      </c>
+      <c r="L27" s="8" t="s">
+        <v>184</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -4077,9 +4999,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P28"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5409,10 +6329,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5567,6 +6487,26 @@
         <v>100</v>
       </c>
     </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>186</v>
+      </c>
+      <c r="B9">
+        <v>0.90949555999999998</v>
+      </c>
+      <c r="C9">
+        <v>9.8647730000000003E-2</v>
+      </c>
+      <c r="D9">
+        <v>-8.1948799999999999E-3</v>
+      </c>
+      <c r="E9" s="8">
+        <v>0</v>
+      </c>
+      <c r="F9" s="8">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -5577,13 +6517,123 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="49.140625" style="8" customWidth="1"/>
+    <col min="2" max="4" width="9.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" style="8" customWidth="1"/>
+    <col min="6" max="6" width="8.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="45.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="8"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="B4" s="8">
+        <v>1</v>
+      </c>
+      <c r="C4" s="8">
+        <v>0</v>
+      </c>
+      <c r="D4" s="8">
+        <v>0</v>
+      </c>
+      <c r="E4" s="8">
+        <v>0</v>
+      </c>
+      <c r="F4" s="8">
+        <v>-100</v>
+      </c>
+      <c r="G4" s="8">
+        <v>100</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="B5" s="8">
+        <v>1</v>
+      </c>
+      <c r="C5" s="8">
+        <v>0</v>
+      </c>
+      <c r="D5" s="8">
+        <v>0</v>
+      </c>
+      <c r="E5" s="8">
+        <v>0</v>
+      </c>
+      <c r="F5" s="8">
+        <v>-100</v>
+      </c>
+      <c r="G5" s="8">
+        <v>100</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>184</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="5" ySplit="3" topLeftCell="F4" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G1" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="F32" sqref="F32"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7149,4 +8199,382 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AE8"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.28515625" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" style="8" customWidth="1"/>
+    <col min="4" max="4" width="23.5703125" customWidth="1"/>
+    <col min="5" max="6" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="30" width="5.7109375" style="10" customWidth="1"/>
+    <col min="31" max="31" width="53.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="J3" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="K3" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="L3" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="M3" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="N3" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="O3" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="P3" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="Q3" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="R3" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="S3" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="T3" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="U3" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="V3" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="W3" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="X3" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="Y3" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="Z3" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="AA3" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="AB3" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="AC3" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="AD3" s="11" t="s">
+        <v>178</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>151</v>
+      </c>
+      <c r="B4" t="s">
+        <v>148</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="D4" t="s">
+        <v>152</v>
+      </c>
+      <c r="E4" s="9">
+        <v>41640</v>
+      </c>
+      <c r="F4" s="9">
+        <v>42004</v>
+      </c>
+      <c r="G4" s="12">
+        <v>0</v>
+      </c>
+      <c r="H4" s="12">
+        <v>0</v>
+      </c>
+      <c r="I4" s="12">
+        <v>0</v>
+      </c>
+      <c r="J4" s="12">
+        <v>0</v>
+      </c>
+      <c r="K4" s="12">
+        <v>0</v>
+      </c>
+      <c r="L4" s="12">
+        <v>0</v>
+      </c>
+      <c r="M4" s="12">
+        <v>0.27</v>
+      </c>
+      <c r="N4" s="12">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="O4" s="12">
+        <v>0.64</v>
+      </c>
+      <c r="P4" s="12">
+        <v>0.64</v>
+      </c>
+      <c r="Q4" s="12">
+        <v>0.82</v>
+      </c>
+      <c r="R4" s="12">
+        <v>1</v>
+      </c>
+      <c r="S4" s="12">
+        <v>0.91</v>
+      </c>
+      <c r="T4" s="12">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="U4" s="12">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="V4" s="12">
+        <v>0.73</v>
+      </c>
+      <c r="W4" s="12">
+        <v>0.37</v>
+      </c>
+      <c r="X4" s="12">
+        <v>0.37</v>
+      </c>
+      <c r="Y4" s="12">
+        <v>0.18</v>
+      </c>
+      <c r="Z4" s="12">
+        <v>0.27</v>
+      </c>
+      <c r="AA4" s="12">
+        <v>0.09</v>
+      </c>
+      <c r="AB4" s="12">
+        <v>0</v>
+      </c>
+      <c r="AC4" s="12">
+        <v>0</v>
+      </c>
+      <c r="AD4" s="12">
+        <v>0</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="E5" s="9">
+        <v>41640</v>
+      </c>
+      <c r="F5" s="9">
+        <v>42004</v>
+      </c>
+      <c r="G5" s="12">
+        <v>0</v>
+      </c>
+      <c r="H5" s="12">
+        <v>0</v>
+      </c>
+      <c r="I5" s="12">
+        <v>0</v>
+      </c>
+      <c r="J5" s="12">
+        <v>0</v>
+      </c>
+      <c r="K5" s="12">
+        <v>0</v>
+      </c>
+      <c r="L5" s="12">
+        <v>0</v>
+      </c>
+      <c r="M5" s="12">
+        <v>0</v>
+      </c>
+      <c r="N5" s="12">
+        <v>0</v>
+      </c>
+      <c r="O5" s="12">
+        <v>0</v>
+      </c>
+      <c r="P5" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="12">
+        <v>0</v>
+      </c>
+      <c r="R5" s="12">
+        <v>0</v>
+      </c>
+      <c r="S5" s="12">
+        <v>0</v>
+      </c>
+      <c r="T5" s="12">
+        <v>0</v>
+      </c>
+      <c r="U5" s="12">
+        <v>0</v>
+      </c>
+      <c r="V5" s="12">
+        <v>0</v>
+      </c>
+      <c r="W5" s="12">
+        <v>0</v>
+      </c>
+      <c r="X5" s="12">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="12">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="12">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="12">
+        <v>0</v>
+      </c>
+      <c r="AB5" s="12">
+        <v>0</v>
+      </c>
+      <c r="AC5" s="12">
+        <v>0</v>
+      </c>
+      <c r="AD5" s="12">
+        <v>0</v>
+      </c>
+      <c r="AE5" s="8" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="G7"/>
+      <c r="H7"/>
+      <c r="I7"/>
+      <c r="J7"/>
+      <c r="K7"/>
+      <c r="L7"/>
+      <c r="M7"/>
+      <c r="N7"/>
+      <c r="O7"/>
+      <c r="P7"/>
+      <c r="Q7"/>
+      <c r="R7"/>
+      <c r="S7"/>
+      <c r="T7"/>
+      <c r="U7"/>
+      <c r="V7"/>
+      <c r="W7"/>
+      <c r="X7"/>
+      <c r="Y7"/>
+      <c r="Z7"/>
+      <c r="AA7"/>
+      <c r="AB7"/>
+      <c r="AC7"/>
+      <c r="AD7"/>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="G8"/>
+      <c r="H8"/>
+      <c r="I8"/>
+      <c r="J8"/>
+      <c r="K8"/>
+      <c r="L8"/>
+      <c r="M8"/>
+      <c r="N8"/>
+      <c r="O8"/>
+      <c r="P8"/>
+      <c r="Q8"/>
+      <c r="R8"/>
+      <c r="S8"/>
+      <c r="T8"/>
+      <c r="U8"/>
+      <c r="V8"/>
+      <c r="W8"/>
+      <c r="X8"/>
+      <c r="Y8"/>
+      <c r="Z8"/>
+      <c r="AA8"/>
+      <c r="AB8"/>
+      <c r="AC8"/>
+      <c r="AD8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update the chiller and 2 speed DX coil lookups
</commit_message>
<xml_diff>
--- a/create_DOE_prototype_building/resources/standards data/HVAC Standards/OpenStudio_HVAC_Standards.xlsx
+++ b/create_DOE_prototype_building/resources/standards data/HVAC Standards/OpenStudio_HVAC_Standards.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="23955" windowHeight="11820" activeTab="6"/>
+    <workbookView xWindow="480" yWindow="30" windowWidth="23955" windowHeight="11820"/>
   </bookViews>
   <sheets>
     <sheet name="PrototypeInputs" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="926" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1061" uniqueCount="198">
   <si>
     <t>Template</t>
   </si>
@@ -607,6 +607,15 @@
   </si>
   <si>
     <t>Each row represents a cubic curve used to describe HVAC component performance</t>
+  </si>
+  <si>
+    <t>ASHRAE 169-2006-3B</t>
+  </si>
+  <si>
+    <t>ASHRAE 169-2006-4A</t>
+  </si>
+  <si>
+    <t>ASHRAE 169-2006-5A</t>
   </si>
 </sst>
 </file>
@@ -720,62 +729,6 @@
   </cellStyles>
   <dxfs count="46">
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -851,13 +804,69 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="171" formatCode="m/d"/>
+      <numFmt numFmtId="166" formatCode="m/d"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.0%"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -870,8 +879,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A3:U9" totalsRowShown="0" headerRowDxfId="17">
-  <autoFilter ref="A3:U9"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A3:U27" totalsRowShown="0" headerRowDxfId="45">
+  <autoFilter ref="A3:U27"/>
   <tableColumns count="21">
     <tableColumn id="1" name="Template"/>
     <tableColumn id="2" name="Climate Zone"/>
@@ -920,24 +929,24 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table58" displayName="Table58" ref="A3:O63" totalsRowShown="0" headerRowDxfId="2" dataDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table58" displayName="Table58" ref="A3:O63" totalsRowShown="0" headerRowDxfId="44" dataDxfId="43">
   <autoFilter ref="A3:O63"/>
   <tableColumns count="15">
-    <tableColumn id="1" name="Template" dataDxfId="15"/>
-    <tableColumn id="2" name="Cooling Type" dataDxfId="14"/>
-    <tableColumn id="6" name="Heating Type" dataDxfId="13"/>
-    <tableColumn id="8" name="Subcategory" dataDxfId="12"/>
-    <tableColumn id="9" name="Minimum Capacity (Btu/hr)" dataDxfId="11" dataCellStyle="Comma"/>
-    <tableColumn id="7" name="Maximum Capacity (Btu/hr)" dataDxfId="10" dataCellStyle="Comma"/>
-    <tableColumn id="10" name="Minimum SEER" dataDxfId="9"/>
-    <tableColumn id="12" name="Minimum EER" dataDxfId="8"/>
-    <tableColumn id="11" name="Minimum IPLV" dataDxfId="7"/>
-    <tableColumn id="3" name="COOL-CAP-FT" dataDxfId="6"/>
-    <tableColumn id="4" name="COOL-CAP-FFLOW" dataDxfId="5"/>
-    <tableColumn id="15" name="COOL-EIR-FT" dataDxfId="0"/>
-    <tableColumn id="14" name="COOL-EIR-FFLOW" dataDxfId="1"/>
-    <tableColumn id="5" name="COOL-PLF-FPLR" dataDxfId="4"/>
-    <tableColumn id="13" name="Notes" dataDxfId="3"/>
+    <tableColumn id="1" name="Template" dataDxfId="42"/>
+    <tableColumn id="2" name="Cooling Type" dataDxfId="41"/>
+    <tableColumn id="6" name="Heating Type" dataDxfId="40"/>
+    <tableColumn id="8" name="Subcategory" dataDxfId="39"/>
+    <tableColumn id="9" name="Minimum Capacity (Btu/hr)" dataDxfId="38" dataCellStyle="Comma"/>
+    <tableColumn id="7" name="Maximum Capacity (Btu/hr)" dataDxfId="37" dataCellStyle="Comma"/>
+    <tableColumn id="10" name="Minimum SEER" dataDxfId="36"/>
+    <tableColumn id="12" name="Minimum EER" dataDxfId="35"/>
+    <tableColumn id="11" name="Minimum IPLV" dataDxfId="34"/>
+    <tableColumn id="3" name="COOL-CAP-FT" dataDxfId="33"/>
+    <tableColumn id="4" name="COOL-CAP-FFLOW" dataDxfId="32"/>
+    <tableColumn id="15" name="COOL-EIR-FT" dataDxfId="31"/>
+    <tableColumn id="14" name="COOL-EIR-FFLOW" dataDxfId="30"/>
+    <tableColumn id="5" name="COOL-PLF-FPLR" dataDxfId="29"/>
+    <tableColumn id="13" name="Notes" dataDxfId="28"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1030,8 +1039,8 @@
     <tableColumn id="2" name="Number of Poles"/>
     <tableColumn id="6" name="Type"/>
     <tableColumn id="9" name="Minimum Capacity (HP)"/>
-    <tableColumn id="7" name="Maximum Capacity (HP)" dataDxfId="45"/>
-    <tableColumn id="10" name="Nominal Full Load Efficiency" dataDxfId="44" dataCellStyle="Percent"/>
+    <tableColumn id="7" name="Maximum Capacity (HP)" dataDxfId="27"/>
+    <tableColumn id="10" name="Nominal Full Load Efficiency" dataDxfId="26" dataCellStyle="Percent"/>
     <tableColumn id="5" name="Notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1046,32 +1055,32 @@
     <tableColumn id="2" name="Type"/>
     <tableColumn id="31" name="Units"/>
     <tableColumn id="6" name="Day Types"/>
-    <tableColumn id="9" name="Start Date" dataDxfId="43"/>
-    <tableColumn id="7" name="End Date" dataDxfId="42"/>
-    <tableColumn id="10" name="Hr 1" dataDxfId="41" dataCellStyle="Percent"/>
-    <tableColumn id="5" name="Hr 2" dataDxfId="40" dataCellStyle="Percent"/>
-    <tableColumn id="3" name="Hr 3" dataDxfId="39" dataCellStyle="Percent"/>
-    <tableColumn id="4" name="Hr 4" dataDxfId="38" dataCellStyle="Percent"/>
-    <tableColumn id="8" name="Hr 5" dataDxfId="37" dataCellStyle="Percent"/>
-    <tableColumn id="11" name="Hr 6" dataDxfId="36" dataCellStyle="Percent"/>
-    <tableColumn id="12" name="Hr 7" dataDxfId="35" dataCellStyle="Percent"/>
-    <tableColumn id="13" name="Hr 8" dataDxfId="34" dataCellStyle="Percent"/>
-    <tableColumn id="14" name="Hr 9" dataDxfId="33" dataCellStyle="Percent"/>
-    <tableColumn id="15" name="Hr 10" dataDxfId="32" dataCellStyle="Percent"/>
-    <tableColumn id="16" name="Hr 11" dataDxfId="31" dataCellStyle="Percent"/>
-    <tableColumn id="17" name="Hr 12" dataDxfId="30" dataCellStyle="Percent"/>
-    <tableColumn id="18" name="Hr 13" dataDxfId="29" dataCellStyle="Percent"/>
-    <tableColumn id="19" name="Hr 14" dataDxfId="28" dataCellStyle="Percent"/>
-    <tableColumn id="20" name="Hr 15" dataDxfId="27" dataCellStyle="Percent"/>
-    <tableColumn id="21" name="Hr 16" dataDxfId="26" dataCellStyle="Percent"/>
-    <tableColumn id="22" name="Hr 17" dataDxfId="25" dataCellStyle="Percent"/>
-    <tableColumn id="23" name="Hr 18" dataDxfId="24" dataCellStyle="Percent"/>
-    <tableColumn id="24" name="Hr 19" dataDxfId="23" dataCellStyle="Percent"/>
-    <tableColumn id="25" name="Hr 20" dataDxfId="22" dataCellStyle="Percent"/>
-    <tableColumn id="26" name="Hr 21" dataDxfId="21" dataCellStyle="Percent"/>
-    <tableColumn id="27" name="Hr 22" dataDxfId="20" dataCellStyle="Percent"/>
-    <tableColumn id="28" name="Hr 23" dataDxfId="19" dataCellStyle="Percent"/>
-    <tableColumn id="29" name="Hr 24" dataDxfId="18" dataCellStyle="Percent"/>
+    <tableColumn id="9" name="Start Date" dataDxfId="25"/>
+    <tableColumn id="7" name="End Date" dataDxfId="24"/>
+    <tableColumn id="10" name="Hr 1" dataDxfId="23" dataCellStyle="Percent"/>
+    <tableColumn id="5" name="Hr 2" dataDxfId="22" dataCellStyle="Percent"/>
+    <tableColumn id="3" name="Hr 3" dataDxfId="21" dataCellStyle="Percent"/>
+    <tableColumn id="4" name="Hr 4" dataDxfId="20" dataCellStyle="Percent"/>
+    <tableColumn id="8" name="Hr 5" dataDxfId="19" dataCellStyle="Percent"/>
+    <tableColumn id="11" name="Hr 6" dataDxfId="18" dataCellStyle="Percent"/>
+    <tableColumn id="12" name="Hr 7" dataDxfId="17" dataCellStyle="Percent"/>
+    <tableColumn id="13" name="Hr 8" dataDxfId="16" dataCellStyle="Percent"/>
+    <tableColumn id="14" name="Hr 9" dataDxfId="15" dataCellStyle="Percent"/>
+    <tableColumn id="15" name="Hr 10" dataDxfId="14" dataCellStyle="Percent"/>
+    <tableColumn id="16" name="Hr 11" dataDxfId="13" dataCellStyle="Percent"/>
+    <tableColumn id="17" name="Hr 12" dataDxfId="12" dataCellStyle="Percent"/>
+    <tableColumn id="18" name="Hr 13" dataDxfId="11" dataCellStyle="Percent"/>
+    <tableColumn id="19" name="Hr 14" dataDxfId="10" dataCellStyle="Percent"/>
+    <tableColumn id="20" name="Hr 15" dataDxfId="9" dataCellStyle="Percent"/>
+    <tableColumn id="21" name="Hr 16" dataDxfId="8" dataCellStyle="Percent"/>
+    <tableColumn id="22" name="Hr 17" dataDxfId="7" dataCellStyle="Percent"/>
+    <tableColumn id="23" name="Hr 18" dataDxfId="6" dataCellStyle="Percent"/>
+    <tableColumn id="24" name="Hr 19" dataDxfId="5" dataCellStyle="Percent"/>
+    <tableColumn id="25" name="Hr 20" dataDxfId="4" dataCellStyle="Percent"/>
+    <tableColumn id="26" name="Hr 21" dataDxfId="3" dataCellStyle="Percent"/>
+    <tableColumn id="27" name="Hr 22" dataDxfId="2" dataCellStyle="Percent"/>
+    <tableColumn id="28" name="Hr 23" dataDxfId="1" dataCellStyle="Percent"/>
+    <tableColumn id="29" name="Hr 24" dataDxfId="0" dataCellStyle="Percent"/>
     <tableColumn id="30" name="Notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1365,13 +1374,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U9"/>
+  <dimension ref="A1:U27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="N4" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A16" sqref="A16"/>
+      <selection pane="bottomRight" activeCell="D13" sqref="D13:P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1558,147 +1567,849 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="1:21" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>106</v>
+      <c r="B7" s="8" t="s">
+        <v>195</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="I7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="H7" s="8">
+        <v>470</v>
+      </c>
+      <c r="I7" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J7" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="K7" t="b">
-        <v>0</v>
-      </c>
-      <c r="M7">
-        <v>2766</v>
-      </c>
-      <c r="N7">
-        <v>40</v>
-      </c>
-      <c r="O7" t="s">
-        <v>143</v>
-      </c>
-      <c r="P7" s="6">
-        <v>2883000</v>
-      </c>
-      <c r="Q7">
-        <v>140</v>
-      </c>
-      <c r="R7" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="S7">
-        <v>0.05</v>
-      </c>
-      <c r="T7">
-        <v>110</v>
-      </c>
-      <c r="U7">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    </row>
+    <row r="8" spans="1:21" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>106</v>
+      <c r="B8" s="8" t="s">
+        <v>195</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="I8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="H8" s="8">
+        <v>470</v>
+      </c>
+      <c r="I8" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="J8" t="s">
+      <c r="J8" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="K8" t="b">
-        <v>0</v>
-      </c>
-      <c r="M8">
-        <v>2766</v>
-      </c>
-      <c r="N8">
-        <v>40</v>
-      </c>
-      <c r="O8" t="s">
-        <v>143</v>
-      </c>
-      <c r="P8" s="6">
-        <v>2883000</v>
-      </c>
-      <c r="Q8">
-        <v>140</v>
-      </c>
-      <c r="R8" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="S8" s="8">
-        <v>0.05</v>
-      </c>
-      <c r="T8" s="8">
-        <v>110</v>
-      </c>
-      <c r="U8" s="8">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:21" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="H9" s="8">
+        <v>470</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="K9" s="8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="H10" s="8">
+        <v>470</v>
+      </c>
+      <c r="I10" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="J10" s="8" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="H11" s="8">
+        <v>470</v>
+      </c>
+      <c r="I11" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="J11" s="8" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="H12" s="8">
+        <v>470</v>
+      </c>
+      <c r="I12" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="J12" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="K12" s="8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="H13" s="8">
+        <v>470</v>
+      </c>
+      <c r="I13" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="J13" s="8" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="H14" s="8">
+        <v>470</v>
+      </c>
+      <c r="I14" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="J14" s="8" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="H15" s="8">
+        <v>470</v>
+      </c>
+      <c r="I15" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="J15" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="K15" s="8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C16" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I16" t="s">
+        <v>132</v>
+      </c>
+      <c r="J16" t="s">
+        <v>130</v>
+      </c>
+      <c r="K16" t="b">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>2766</v>
+      </c>
+      <c r="N16">
+        <v>40</v>
+      </c>
+      <c r="O16" t="s">
+        <v>143</v>
+      </c>
+      <c r="P16" s="6">
+        <v>2883000</v>
+      </c>
+      <c r="Q16">
+        <v>140</v>
+      </c>
+      <c r="R16" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="S16">
+        <v>0.05</v>
+      </c>
+      <c r="T16">
+        <v>110</v>
+      </c>
+      <c r="U16">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="I17" t="s">
+        <v>132</v>
+      </c>
+      <c r="J17" t="s">
+        <v>130</v>
+      </c>
+      <c r="K17" t="b">
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <v>2766</v>
+      </c>
+      <c r="N17">
+        <v>40</v>
+      </c>
+      <c r="O17" t="s">
+        <v>143</v>
+      </c>
+      <c r="P17" s="6">
+        <v>2883000</v>
+      </c>
+      <c r="Q17">
+        <v>140</v>
+      </c>
+      <c r="R17" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="S17" s="8">
+        <v>0.05</v>
+      </c>
+      <c r="T17" s="8">
+        <v>110</v>
+      </c>
+      <c r="U17" s="8">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="I18" t="s">
         <v>134</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J18" t="s">
         <v>134</v>
       </c>
-      <c r="K9" t="b">
-        <v>0</v>
-      </c>
-      <c r="L9">
+      <c r="K18" t="b">
+        <v>0</v>
+      </c>
+      <c r="L18">
         <v>896.07</v>
       </c>
-      <c r="M9">
+      <c r="M18">
         <v>40.54</v>
       </c>
-      <c r="N9">
+      <c r="N18">
         <v>40</v>
       </c>
-      <c r="O9" t="s">
+      <c r="O18" t="s">
         <v>139</v>
       </c>
-      <c r="P9" s="6">
+      <c r="P18" s="6">
         <v>40000</v>
       </c>
-      <c r="Q9" s="8">
+      <c r="Q18" s="8">
         <v>140</v>
       </c>
-      <c r="R9" s="8" t="s">
+      <c r="R18" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="S9">
+      <c r="S18">
         <v>6.4000000000000001E-2</v>
       </c>
-      <c r="T9">
+      <c r="T18">
         <v>120</v>
       </c>
-      <c r="U9">
+      <c r="U18">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="I19" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="J19" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="K19" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="M19" s="8">
+        <v>2766</v>
+      </c>
+      <c r="N19" s="8">
+        <v>40</v>
+      </c>
+      <c r="O19" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="P19" s="6">
+        <v>2883000</v>
+      </c>
+      <c r="Q19" s="8">
+        <v>140</v>
+      </c>
+      <c r="R19" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="S19" s="8">
+        <v>0.05</v>
+      </c>
+      <c r="T19" s="8">
+        <v>110</v>
+      </c>
+      <c r="U19" s="8">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="I20" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="J20" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="K20" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="M20" s="8">
+        <v>2766</v>
+      </c>
+      <c r="N20" s="8">
+        <v>40</v>
+      </c>
+      <c r="O20" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="P20" s="6">
+        <v>2883000</v>
+      </c>
+      <c r="Q20" s="8">
+        <v>140</v>
+      </c>
+      <c r="R20" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="S20" s="8">
+        <v>0.05</v>
+      </c>
+      <c r="T20" s="8">
+        <v>110</v>
+      </c>
+      <c r="U20" s="8">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>195</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="I21" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="J21" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="K21" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="L21" s="8">
+        <v>896.07</v>
+      </c>
+      <c r="M21" s="8">
+        <v>40.54</v>
+      </c>
+      <c r="N21" s="8">
+        <v>40</v>
+      </c>
+      <c r="O21" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="P21" s="6">
+        <v>40000</v>
+      </c>
+      <c r="Q21" s="8">
+        <v>140</v>
+      </c>
+      <c r="R21" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="S21" s="8">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="T21" s="8">
+        <v>120</v>
+      </c>
+      <c r="U21" s="8">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="I22" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="J22" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="K22" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="M22" s="8">
+        <v>2766</v>
+      </c>
+      <c r="N22" s="8">
+        <v>40</v>
+      </c>
+      <c r="O22" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="P22" s="6">
+        <v>2883000</v>
+      </c>
+      <c r="Q22" s="8">
+        <v>140</v>
+      </c>
+      <c r="R22" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="S22" s="8">
+        <v>0.05</v>
+      </c>
+      <c r="T22" s="8">
+        <v>110</v>
+      </c>
+      <c r="U22" s="8">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="I23" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="J23" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="K23" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="M23" s="8">
+        <v>2766</v>
+      </c>
+      <c r="N23" s="8">
+        <v>40</v>
+      </c>
+      <c r="O23" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="P23" s="6">
+        <v>2883000</v>
+      </c>
+      <c r="Q23" s="8">
+        <v>140</v>
+      </c>
+      <c r="R23" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="S23" s="8">
+        <v>0.05</v>
+      </c>
+      <c r="T23" s="8">
+        <v>110</v>
+      </c>
+      <c r="U23" s="8">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="I24" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="J24" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="K24" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="L24" s="8">
+        <v>896.07</v>
+      </c>
+      <c r="M24" s="8">
+        <v>40.54</v>
+      </c>
+      <c r="N24" s="8">
+        <v>40</v>
+      </c>
+      <c r="O24" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="P24" s="6">
+        <v>40000</v>
+      </c>
+      <c r="Q24" s="8">
+        <v>140</v>
+      </c>
+      <c r="R24" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="S24" s="8">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="T24" s="8">
+        <v>120</v>
+      </c>
+      <c r="U24" s="8">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="I25" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="J25" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="K25" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="M25" s="8">
+        <v>2766</v>
+      </c>
+      <c r="N25" s="8">
+        <v>40</v>
+      </c>
+      <c r="O25" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="P25" s="6">
+        <v>2883000</v>
+      </c>
+      <c r="Q25" s="8">
+        <v>140</v>
+      </c>
+      <c r="R25" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="S25" s="8">
+        <v>0.05</v>
+      </c>
+      <c r="T25" s="8">
+        <v>110</v>
+      </c>
+      <c r="U25" s="8">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="I26" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="J26" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="K26" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="M26" s="8">
+        <v>2766</v>
+      </c>
+      <c r="N26" s="8">
+        <v>40</v>
+      </c>
+      <c r="O26" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="P26" s="6">
+        <v>2883000</v>
+      </c>
+      <c r="Q26" s="8">
+        <v>140</v>
+      </c>
+      <c r="R26" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="S26" s="8">
+        <v>0.05</v>
+      </c>
+      <c r="T26" s="8">
+        <v>110</v>
+      </c>
+      <c r="U26" s="8">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="I27" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="J27" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="K27" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="L27" s="8">
+        <v>896.07</v>
+      </c>
+      <c r="M27" s="8">
+        <v>40.54</v>
+      </c>
+      <c r="N27" s="8">
+        <v>40</v>
+      </c>
+      <c r="O27" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="P27" s="6">
+        <v>40000</v>
+      </c>
+      <c r="Q27" s="8">
+        <v>140</v>
+      </c>
+      <c r="R27" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="S27" s="8">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="T27" s="8">
+        <v>120</v>
+      </c>
+      <c r="U27" s="8">
         <v>131</v>
       </c>
     </row>
@@ -6519,7 +7230,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Adds unitary equipment fan and supplemental htg type
</commit_message>
<xml_diff>
--- a/create_DOE_prototype_building/resources/standards data/HVAC Standards/OpenStudio_HVAC_Standards.xlsx
+++ b/create_DOE_prototype_building/resources/standards data/HVAC Standards/OpenStudio_HVAC_Standards.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1061" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1091" uniqueCount="202">
   <si>
     <t>Template</t>
   </si>
@@ -616,6 +616,18 @@
   </si>
   <si>
     <t>ASHRAE 169-2006-5A</t>
+  </si>
+  <si>
+    <t>Unitary AC Fan Type</t>
+  </si>
+  <si>
+    <t>ConstantVolume</t>
+  </si>
+  <si>
+    <t>Cycling</t>
+  </si>
+  <si>
+    <t>Unitary AC Supplemental Heating Type</t>
   </si>
 </sst>
 </file>
@@ -879,9 +891,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A3:U27" totalsRowShown="0" headerRowDxfId="45">
-  <autoFilter ref="A3:U27"/>
-  <tableColumns count="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A3:W27" totalsRowShown="0" headerRowDxfId="45">
+  <autoFilter ref="A3:W27"/>
+  <tableColumns count="23">
     <tableColumn id="1" name="Template"/>
     <tableColumn id="2" name="Climate Zone"/>
     <tableColumn id="3" name="BuildingType"/>
@@ -903,6 +915,8 @@
     <tableColumn id="19" name="Service Water Peak FlowRate (gal/min)"/>
     <tableColumn id="20" name="Water Use Temperature (F)"/>
     <tableColumn id="21" name="Service Water Temperature at Fixture (F)"/>
+    <tableColumn id="22" name="Unitary AC Fan Type"/>
+    <tableColumn id="23" name="Unitary AC Supplemental Heating Type"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1374,13 +1388,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U27"/>
+  <dimension ref="A1:W27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="M4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D13" sqref="D13:P15"/>
+      <selection pane="bottomRight" activeCell="X27" sqref="X27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1405,14 +1419,16 @@
     <col min="18" max="18" width="26.140625" customWidth="1"/>
     <col min="19" max="19" width="14.7109375" customWidth="1"/>
     <col min="20" max="20" width="17.28515625" customWidth="1"/>
+    <col min="22" max="22" width="16.5703125" customWidth="1"/>
+    <col min="23" max="23" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="3" spans="1:21" s="4" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" s="4" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -1476,8 +1492,14 @@
       <c r="U3" s="4" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V3" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="W3" s="4" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1505,8 +1527,11 @@
       <c r="J4" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V4" s="8" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1534,8 +1559,12 @@
       <c r="J5" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V5" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="W5" s="8"/>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
@@ -1566,8 +1595,12 @@
       <c r="K6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:21" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V6" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="W6" s="8"/>
+    </row>
+    <row r="7" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>8</v>
       </c>
@@ -1595,8 +1628,11 @@
       <c r="J7" s="8" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="8" spans="1:21" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V7" s="8" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>7</v>
       </c>
@@ -1624,8 +1660,11 @@
       <c r="J8" s="8" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="9" spans="1:21" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V8" s="8" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>2</v>
       </c>
@@ -1656,8 +1695,11 @@
       <c r="K9" s="8" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:21" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V9" s="8" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>8</v>
       </c>
@@ -1685,8 +1727,11 @@
       <c r="J10" s="8" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="11" spans="1:21" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V10" s="8" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>7</v>
       </c>
@@ -1714,8 +1759,11 @@
       <c r="J11" s="8" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="12" spans="1:21" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V11" s="8" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
@@ -1746,8 +1794,11 @@
       <c r="K12" s="8" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:21" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V12" s="8" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>8</v>
       </c>
@@ -1775,8 +1826,11 @@
       <c r="J13" s="8" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="14" spans="1:21" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V13" s="8" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>7</v>
       </c>
@@ -1804,8 +1858,11 @@
       <c r="J14" s="8" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="15" spans="1:21" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V14" s="8" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>2</v>
       </c>
@@ -1836,8 +1893,11 @@
       <c r="K15" s="8" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V15" s="8" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -1883,8 +1943,11 @@
       <c r="U16">
         <v>110</v>
       </c>
-    </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V16" s="8" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -1930,8 +1993,11 @@
       <c r="U17" s="8">
         <v>110</v>
       </c>
-    </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V17" s="8" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>2</v>
       </c>
@@ -1980,8 +2046,14 @@
       <c r="U18">
         <v>131</v>
       </c>
-    </row>
-    <row r="19" spans="1:21" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V18" t="s">
+        <v>200</v>
+      </c>
+      <c r="W18" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>8</v>
       </c>
@@ -2027,8 +2099,11 @@
       <c r="U19" s="8">
         <v>110</v>
       </c>
-    </row>
-    <row r="20" spans="1:21" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V19" s="8" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>7</v>
       </c>
@@ -2074,8 +2149,11 @@
       <c r="U20" s="8">
         <v>110</v>
       </c>
-    </row>
-    <row r="21" spans="1:21" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V20" s="8" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>2</v>
       </c>
@@ -2124,8 +2202,14 @@
       <c r="U21" s="8">
         <v>131</v>
       </c>
-    </row>
-    <row r="22" spans="1:21" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V21" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="W21" s="8" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
         <v>8</v>
       </c>
@@ -2171,8 +2255,11 @@
       <c r="U22" s="8">
         <v>110</v>
       </c>
-    </row>
-    <row r="23" spans="1:21" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V22" s="8" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>7</v>
       </c>
@@ -2218,8 +2305,11 @@
       <c r="U23" s="8">
         <v>110</v>
       </c>
-    </row>
-    <row r="24" spans="1:21" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V23" s="8" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>2</v>
       </c>
@@ -2268,8 +2358,14 @@
       <c r="U24" s="8">
         <v>131</v>
       </c>
-    </row>
-    <row r="25" spans="1:21" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V24" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="W24" s="8" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
         <v>8</v>
       </c>
@@ -2315,8 +2411,11 @@
       <c r="U25" s="8">
         <v>110</v>
       </c>
-    </row>
-    <row r="26" spans="1:21" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V25" s="8" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
         <v>7</v>
       </c>
@@ -2362,8 +2461,11 @@
       <c r="U26" s="8">
         <v>110</v>
       </c>
-    </row>
-    <row r="27" spans="1:21" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V26" s="8" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>2</v>
       </c>
@@ -2411,6 +2513,12 @@
       </c>
       <c r="U27" s="8">
         <v>131</v>
+      </c>
+      <c r="V27" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="W27" s="8" t="s">
+        <v>130</v>
       </c>
     </row>
   </sheetData>

</xml_diff>